<commit_message>
creating histogram for the matching graphs from class A (test)
</commit_message>
<xml_diff>
--- a/letter_results/pruning_cost_1.6_dist_0.9_train/MG_A_end_df.xlsx
+++ b/letter_results/pruning_cost_1.6_dist_0.9_train/MG_A_end_df.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zhaox\PycharmProjects\BachelorThesis\letter_results\pruning_cost_1.6_dist_0.9_train\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10FC7F67-2C51-4B2D-A5BF-06091A98B078}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A62B9851-D646-4631-83F2-004F55D2B354}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -448,254 +448,6 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strRef>
-              <c:f>Sheet1!$A$2:$A$81</c:f>
-              <c:strCache>
-                <c:ptCount val="80"/>
-                <c:pt idx="0">
-                  <c:v>21_63AP1_0007_matching_graph</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>23_138AP1_0007_matching_graph</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>25_864AP1_0007_matching_graph</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>27_878AP1_0007_matching_graph</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>29_915AP1_0007_matching_graph</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>31_974AP1_0007_matching_graph</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>33_197AP1_0007_matching_graph</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>35_205AP1_0007_matching_graph</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>37_219AP1_0007_matching_graph</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>39_236AP1_0007_matching_graph</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>41_258AP1_0007_matching_graph</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>43_267AP1_0007_matching_graph</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>45_214AP1_0007_matching_graph</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>47_269AP1_0007_matching_graph</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>49_323AP1_0007_matching_graph</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>50_331AP1_0007_matching_graph</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>51_271AP1_0007_matching_graph</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>52_162AP1_0019_matching_graph</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>53_77AP1_0019_matching_graph</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>54_143AP1_0019_matching_graph</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>55_219AP1_0019_matching_graph</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>56_331AP1_0019_matching_graph</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>57_488AP1_0019_matching_graph</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>58_654AP1_0019_matching_graph</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>59_703AP1_0019_matching_graph</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>60_774AP1_0019_matching_graph</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>61_595AP1_0019_matching_graph</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>62_751AP1_0019_matching_graph</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>63_778AP1_0019_matching_graph</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>64_823AP1_0019_matching_graph</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>65_645AP1_0019_matching_graph</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>66_664AP1_0019_matching_graph</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>18_162AP1_0032_matching_graph</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>19_191AP1_0032_matching_graph</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>20_259AP1_0032_matching_graph</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>22_507AP1_0032_matching_graph</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>24_467AP1_0032_matching_graph</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>26_529AP1_0032_matching_graph</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>28_655AP1_0032_matching_graph</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>30_673AP1_0032_matching_graph</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>32_768AP1_0032_matching_graph</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>34_860AP1_0032_matching_graph</c:v>
-                </c:pt>
-                <c:pt idx="42">
-                  <c:v>36_1012AP1_0032_matching_graph</c:v>
-                </c:pt>
-                <c:pt idx="43">
-                  <c:v>38_1058AP1_0032_matching_graph</c:v>
-                </c:pt>
-                <c:pt idx="44">
-                  <c:v>40_988AP1_0032_matching_graph</c:v>
-                </c:pt>
-                <c:pt idx="45">
-                  <c:v>42_1125AP1_0032_matching_graph</c:v>
-                </c:pt>
-                <c:pt idx="46">
-                  <c:v>44_1111AP1_0032_matching_graph</c:v>
-                </c:pt>
-                <c:pt idx="47">
-                  <c:v>46_1124AP1_0032_matching_graph</c:v>
-                </c:pt>
-                <c:pt idx="48">
-                  <c:v>48_1137AP1_0032_matching_graph</c:v>
-                </c:pt>
-                <c:pt idx="49">
-                  <c:v>0_54AP1_0037_matching_graph</c:v>
-                </c:pt>
-                <c:pt idx="50">
-                  <c:v>10_1057AP1_0037_matching_graph</c:v>
-                </c:pt>
-                <c:pt idx="51">
-                  <c:v>11_1152AP1_0037_matching_graph</c:v>
-                </c:pt>
-                <c:pt idx="52">
-                  <c:v>12_1083AP1_0037_matching_graph</c:v>
-                </c:pt>
-                <c:pt idx="53">
-                  <c:v>13_1129AP1_0037_matching_graph</c:v>
-                </c:pt>
-                <c:pt idx="54">
-                  <c:v>14_1139AP1_0037_matching_graph</c:v>
-                </c:pt>
-                <c:pt idx="55">
-                  <c:v>15_1146AP1_0037_matching_graph</c:v>
-                </c:pt>
-                <c:pt idx="56">
-                  <c:v>16_1155AP1_0037_matching_graph</c:v>
-                </c:pt>
-                <c:pt idx="57">
-                  <c:v>17_1166AP1_0037_matching_graph</c:v>
-                </c:pt>
-                <c:pt idx="58">
-                  <c:v>1_719AP1_0037_matching_graph</c:v>
-                </c:pt>
-                <c:pt idx="59">
-                  <c:v>2_660AP1_0037_matching_graph</c:v>
-                </c:pt>
-                <c:pt idx="60">
-                  <c:v>3_331AP1_0037_matching_graph</c:v>
-                </c:pt>
-                <c:pt idx="61">
-                  <c:v>4_520AP1_0037_matching_graph</c:v>
-                </c:pt>
-                <c:pt idx="62">
-                  <c:v>5_558AP1_0037_matching_graph</c:v>
-                </c:pt>
-                <c:pt idx="63">
-                  <c:v>6_751AP1_0037_matching_graph</c:v>
-                </c:pt>
-                <c:pt idx="64">
-                  <c:v>7_860AP1_0037_matching_graph</c:v>
-                </c:pt>
-                <c:pt idx="65">
-                  <c:v>8_923AP1_0037_matching_graph</c:v>
-                </c:pt>
-                <c:pt idx="66">
-                  <c:v>9_956AP1_0037_matching_graph</c:v>
-                </c:pt>
-                <c:pt idx="67">
-                  <c:v>76_110AP1_0039_matching_graph</c:v>
-                </c:pt>
-                <c:pt idx="68">
-                  <c:v>77_86AP1_0039_matching_graph</c:v>
-                </c:pt>
-                <c:pt idx="69">
-                  <c:v>78_706AP1_0039_matching_graph</c:v>
-                </c:pt>
-                <c:pt idx="70">
-                  <c:v>79_354AP1_0039_matching_graph</c:v>
-                </c:pt>
-                <c:pt idx="71">
-                  <c:v>67_185AP1_0043_matching_graph</c:v>
-                </c:pt>
-                <c:pt idx="72">
-                  <c:v>68_893AP1_0043_matching_graph</c:v>
-                </c:pt>
-                <c:pt idx="73">
-                  <c:v>69_645AP1_0043_matching_graph</c:v>
-                </c:pt>
-                <c:pt idx="74">
-                  <c:v>70_919AP1_0043_matching_graph</c:v>
-                </c:pt>
-                <c:pt idx="75">
-                  <c:v>71_1095AP1_0043_matching_graph</c:v>
-                </c:pt>
-                <c:pt idx="76">
-                  <c:v>72_1138AP1_0043_matching_graph</c:v>
-                </c:pt>
-                <c:pt idx="77">
-                  <c:v>73_1205AP1_0043_matching_graph</c:v>
-                </c:pt>
-                <c:pt idx="78">
-                  <c:v>74_1204AP1_0043_matching_graph</c:v>
-                </c:pt>
-                <c:pt idx="79">
-                  <c:v>75_1210AP1_0043_matching_graph</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
           <c:val>
             <c:numRef>
               <c:f>Sheet1!$B$2:$B$81</c:f>
@@ -703,100 +455,100 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="80"/>
                 <c:pt idx="0">
-                  <c:v>36</c:v>
+                  <c:v>41</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>36</c:v>
+                  <c:v>41</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>36</c:v>
+                  <c:v>41</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>36</c:v>
+                  <c:v>41</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>36</c:v>
+                  <c:v>41</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>36</c:v>
+                  <c:v>41</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>36</c:v>
+                  <c:v>41</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>36</c:v>
+                  <c:v>41</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>36</c:v>
+                  <c:v>41</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>36</c:v>
+                  <c:v>41</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>36</c:v>
+                  <c:v>41</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>36</c:v>
+                  <c:v>41</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>36</c:v>
+                  <c:v>41</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>36</c:v>
+                  <c:v>41</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>36</c:v>
+                  <c:v>41</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>36</c:v>
+                  <c:v>41</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>36</c:v>
+                  <c:v>41</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>34</c:v>
+                  <c:v>41</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>34</c:v>
+                  <c:v>37</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>34</c:v>
+                  <c:v>37</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>34</c:v>
+                  <c:v>37</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>34</c:v>
+                  <c:v>37</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>34</c:v>
+                  <c:v>37</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>34</c:v>
+                  <c:v>37</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>34</c:v>
+                  <c:v>37</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>34</c:v>
+                  <c:v>37</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>34</c:v>
+                  <c:v>37</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>34</c:v>
+                  <c:v>37</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>34</c:v>
+                  <c:v>37</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>34</c:v>
+                  <c:v>37</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>34</c:v>
+                  <c:v>37</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>34</c:v>
+                  <c:v>37</c:v>
                 </c:pt>
                 <c:pt idx="32">
                   <c:v>37</c:v>
@@ -808,100 +560,100 @@
                   <c:v>37</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>37</c:v>
+                  <c:v>36</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>37</c:v>
+                  <c:v>36</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>37</c:v>
+                  <c:v>36</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>37</c:v>
+                  <c:v>36</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>37</c:v>
+                  <c:v>36</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>37</c:v>
+                  <c:v>36</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>37</c:v>
+                  <c:v>36</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>37</c:v>
+                  <c:v>36</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>37</c:v>
+                  <c:v>36</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>37</c:v>
+                  <c:v>36</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>37</c:v>
+                  <c:v>36</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>37</c:v>
+                  <c:v>36</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>37</c:v>
+                  <c:v>36</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>37</c:v>
+                  <c:v>36</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>41</c:v>
+                  <c:v>36</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>41</c:v>
+                  <c:v>36</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>41</c:v>
+                  <c:v>36</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>41</c:v>
+                  <c:v>34</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>41</c:v>
+                  <c:v>34</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>41</c:v>
+                  <c:v>34</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>41</c:v>
+                  <c:v>34</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>41</c:v>
+                  <c:v>34</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>41</c:v>
+                  <c:v>34</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>41</c:v>
+                  <c:v>34</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>41</c:v>
+                  <c:v>34</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>41</c:v>
+                  <c:v>34</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>41</c:v>
+                  <c:v>34</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>41</c:v>
+                  <c:v>34</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>41</c:v>
+                  <c:v>34</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>41</c:v>
+                  <c:v>34</c:v>
                 </c:pt>
                 <c:pt idx="65">
-                  <c:v>41</c:v>
+                  <c:v>34</c:v>
                 </c:pt>
                 <c:pt idx="66">
-                  <c:v>41</c:v>
+                  <c:v>34</c:v>
                 </c:pt>
                 <c:pt idx="67">
                   <c:v>34</c:v>
@@ -947,7 +699,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-DC88-4D0E-95B9-9B0E15769225}"/>
+              <c16:uniqueId val="{00000000-88C1-4D98-BD61-62A660C1FD7E}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -975,254 +727,6 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strRef>
-              <c:f>Sheet1!$A$2:$A$81</c:f>
-              <c:strCache>
-                <c:ptCount val="80"/>
-                <c:pt idx="0">
-                  <c:v>21_63AP1_0007_matching_graph</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>23_138AP1_0007_matching_graph</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>25_864AP1_0007_matching_graph</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>27_878AP1_0007_matching_graph</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>29_915AP1_0007_matching_graph</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>31_974AP1_0007_matching_graph</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>33_197AP1_0007_matching_graph</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>35_205AP1_0007_matching_graph</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>37_219AP1_0007_matching_graph</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>39_236AP1_0007_matching_graph</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>41_258AP1_0007_matching_graph</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>43_267AP1_0007_matching_graph</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>45_214AP1_0007_matching_graph</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>47_269AP1_0007_matching_graph</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>49_323AP1_0007_matching_graph</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>50_331AP1_0007_matching_graph</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>51_271AP1_0007_matching_graph</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>52_162AP1_0019_matching_graph</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>53_77AP1_0019_matching_graph</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>54_143AP1_0019_matching_graph</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>55_219AP1_0019_matching_graph</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>56_331AP1_0019_matching_graph</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>57_488AP1_0019_matching_graph</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>58_654AP1_0019_matching_graph</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>59_703AP1_0019_matching_graph</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>60_774AP1_0019_matching_graph</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>61_595AP1_0019_matching_graph</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>62_751AP1_0019_matching_graph</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>63_778AP1_0019_matching_graph</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>64_823AP1_0019_matching_graph</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>65_645AP1_0019_matching_graph</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>66_664AP1_0019_matching_graph</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>18_162AP1_0032_matching_graph</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>19_191AP1_0032_matching_graph</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>20_259AP1_0032_matching_graph</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>22_507AP1_0032_matching_graph</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>24_467AP1_0032_matching_graph</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>26_529AP1_0032_matching_graph</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>28_655AP1_0032_matching_graph</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>30_673AP1_0032_matching_graph</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>32_768AP1_0032_matching_graph</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>34_860AP1_0032_matching_graph</c:v>
-                </c:pt>
-                <c:pt idx="42">
-                  <c:v>36_1012AP1_0032_matching_graph</c:v>
-                </c:pt>
-                <c:pt idx="43">
-                  <c:v>38_1058AP1_0032_matching_graph</c:v>
-                </c:pt>
-                <c:pt idx="44">
-                  <c:v>40_988AP1_0032_matching_graph</c:v>
-                </c:pt>
-                <c:pt idx="45">
-                  <c:v>42_1125AP1_0032_matching_graph</c:v>
-                </c:pt>
-                <c:pt idx="46">
-                  <c:v>44_1111AP1_0032_matching_graph</c:v>
-                </c:pt>
-                <c:pt idx="47">
-                  <c:v>46_1124AP1_0032_matching_graph</c:v>
-                </c:pt>
-                <c:pt idx="48">
-                  <c:v>48_1137AP1_0032_matching_graph</c:v>
-                </c:pt>
-                <c:pt idx="49">
-                  <c:v>0_54AP1_0037_matching_graph</c:v>
-                </c:pt>
-                <c:pt idx="50">
-                  <c:v>10_1057AP1_0037_matching_graph</c:v>
-                </c:pt>
-                <c:pt idx="51">
-                  <c:v>11_1152AP1_0037_matching_graph</c:v>
-                </c:pt>
-                <c:pt idx="52">
-                  <c:v>12_1083AP1_0037_matching_graph</c:v>
-                </c:pt>
-                <c:pt idx="53">
-                  <c:v>13_1129AP1_0037_matching_graph</c:v>
-                </c:pt>
-                <c:pt idx="54">
-                  <c:v>14_1139AP1_0037_matching_graph</c:v>
-                </c:pt>
-                <c:pt idx="55">
-                  <c:v>15_1146AP1_0037_matching_graph</c:v>
-                </c:pt>
-                <c:pt idx="56">
-                  <c:v>16_1155AP1_0037_matching_graph</c:v>
-                </c:pt>
-                <c:pt idx="57">
-                  <c:v>17_1166AP1_0037_matching_graph</c:v>
-                </c:pt>
-                <c:pt idx="58">
-                  <c:v>1_719AP1_0037_matching_graph</c:v>
-                </c:pt>
-                <c:pt idx="59">
-                  <c:v>2_660AP1_0037_matching_graph</c:v>
-                </c:pt>
-                <c:pt idx="60">
-                  <c:v>3_331AP1_0037_matching_graph</c:v>
-                </c:pt>
-                <c:pt idx="61">
-                  <c:v>4_520AP1_0037_matching_graph</c:v>
-                </c:pt>
-                <c:pt idx="62">
-                  <c:v>5_558AP1_0037_matching_graph</c:v>
-                </c:pt>
-                <c:pt idx="63">
-                  <c:v>6_751AP1_0037_matching_graph</c:v>
-                </c:pt>
-                <c:pt idx="64">
-                  <c:v>7_860AP1_0037_matching_graph</c:v>
-                </c:pt>
-                <c:pt idx="65">
-                  <c:v>8_923AP1_0037_matching_graph</c:v>
-                </c:pt>
-                <c:pt idx="66">
-                  <c:v>9_956AP1_0037_matching_graph</c:v>
-                </c:pt>
-                <c:pt idx="67">
-                  <c:v>76_110AP1_0039_matching_graph</c:v>
-                </c:pt>
-                <c:pt idx="68">
-                  <c:v>77_86AP1_0039_matching_graph</c:v>
-                </c:pt>
-                <c:pt idx="69">
-                  <c:v>78_706AP1_0039_matching_graph</c:v>
-                </c:pt>
-                <c:pt idx="70">
-                  <c:v>79_354AP1_0039_matching_graph</c:v>
-                </c:pt>
-                <c:pt idx="71">
-                  <c:v>67_185AP1_0043_matching_graph</c:v>
-                </c:pt>
-                <c:pt idx="72">
-                  <c:v>68_893AP1_0043_matching_graph</c:v>
-                </c:pt>
-                <c:pt idx="73">
-                  <c:v>69_645AP1_0043_matching_graph</c:v>
-                </c:pt>
-                <c:pt idx="74">
-                  <c:v>70_919AP1_0043_matching_graph</c:v>
-                </c:pt>
-                <c:pt idx="75">
-                  <c:v>71_1095AP1_0043_matching_graph</c:v>
-                </c:pt>
-                <c:pt idx="76">
-                  <c:v>72_1138AP1_0043_matching_graph</c:v>
-                </c:pt>
-                <c:pt idx="77">
-                  <c:v>73_1205AP1_0043_matching_graph</c:v>
-                </c:pt>
-                <c:pt idx="78">
-                  <c:v>74_1204AP1_0043_matching_graph</c:v>
-                </c:pt>
-                <c:pt idx="79">
-                  <c:v>75_1210AP1_0043_matching_graph</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
           <c:val>
             <c:numRef>
               <c:f>Sheet1!$C$2:$C$81</c:f>
@@ -1230,100 +734,100 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="80"/>
                 <c:pt idx="0">
-                  <c:v>14</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>14</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>14</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>14</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>14</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>14</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>14</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>14</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>14</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>14</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>14</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>14</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>14</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>14</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>14</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>14</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>14</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>15</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>15</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>15</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>15</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>15</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>15</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>15</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>15</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>15</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>15</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>15</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>15</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>15</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>15</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>15</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="32">
                   <c:v>12</c:v>
@@ -1335,100 +839,100 @@
                   <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>12</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>12</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>12</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>12</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>12</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>12</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>12</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>12</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>12</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>12</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>12</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>12</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>12</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>12</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>19</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>19</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>19</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>19</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>19</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>19</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>19</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>19</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>19</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>19</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>19</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>19</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>19</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>19</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>19</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>19</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="65">
-                  <c:v>19</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="66">
-                  <c:v>19</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="67">
                   <c:v>19</c:v>
@@ -1474,7 +978,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-DC88-4D0E-95B9-9B0E15769225}"/>
+              <c16:uniqueId val="{00000001-88C1-4D98-BD61-62A660C1FD7E}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1488,17 +992,16 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="1848662591"/>
-        <c:axId val="1848619151"/>
+        <c:axId val="329770224"/>
+        <c:axId val="336061712"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1848662591"/>
+        <c:axId val="329770224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1535,7 +1038,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1848619151"/>
+        <c:crossAx val="336061712"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1543,7 +1046,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1848619151"/>
+        <c:axId val="336061712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1594,7 +1097,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1848662591"/>
+        <c:crossAx val="329770224"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2228,23 +1731,23 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>466724</xdr:colOff>
-      <xdr:row>47</xdr:row>
-      <xdr:rowOff>128586</xdr:rowOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>95250</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>104774</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>571499</xdr:colOff>
-      <xdr:row>65</xdr:row>
-      <xdr:rowOff>57149</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>589650</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>106274</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="3" name="Diagramm 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2F2A9694-250F-49DB-AA1C-A2AA1B34740D}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FA34220A-9CB8-46A2-8A02-A0DA303D916A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2552,13 +2055,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="E72" sqref="E72"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G30" sqref="G30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="3" width="39.85546875" customWidth="1"/>
+    <col min="1" max="1" width="50" customWidth="1"/>
+    <col min="2" max="2" width="18.140625" customWidth="1"/>
+    <col min="3" max="3" width="19.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -2571,359 +2076,359 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>2</v>
+        <v>51</v>
       </c>
       <c r="B2">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="C2">
-        <v>14</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>3</v>
+        <v>52</v>
       </c>
       <c r="B3">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="C3">
-        <v>14</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>4</v>
+        <v>53</v>
       </c>
       <c r="B4">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="C4">
-        <v>14</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>5</v>
+        <v>54</v>
       </c>
       <c r="B5">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="C5">
-        <v>14</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>6</v>
+        <v>55</v>
       </c>
       <c r="B6">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="C6">
-        <v>14</v>
+        <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>7</v>
+        <v>56</v>
       </c>
       <c r="B7">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="C7">
-        <v>14</v>
+        <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>8</v>
+        <v>57</v>
       </c>
       <c r="B8">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="C8">
-        <v>14</v>
+        <v>19</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>9</v>
+        <v>58</v>
       </c>
       <c r="B9">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="C9">
-        <v>14</v>
+        <v>19</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>10</v>
+        <v>59</v>
       </c>
       <c r="B10">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="C10">
-        <v>14</v>
+        <v>19</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>11</v>
+        <v>60</v>
       </c>
       <c r="B11">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="C11">
-        <v>14</v>
+        <v>19</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>12</v>
+        <v>61</v>
       </c>
       <c r="B12">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="C12">
-        <v>14</v>
+        <v>19</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>13</v>
+        <v>62</v>
       </c>
       <c r="B13">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="C13">
-        <v>14</v>
+        <v>19</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>14</v>
+        <v>63</v>
       </c>
       <c r="B14">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="C14">
-        <v>14</v>
+        <v>19</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>15</v>
+        <v>64</v>
       </c>
       <c r="B15">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="C15">
-        <v>14</v>
+        <v>19</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>16</v>
+        <v>65</v>
       </c>
       <c r="B16">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="C16">
-        <v>14</v>
+        <v>19</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>17</v>
+        <v>66</v>
       </c>
       <c r="B17">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="C17">
-        <v>14</v>
+        <v>19</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>18</v>
+        <v>67</v>
       </c>
       <c r="B18">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="C18">
-        <v>14</v>
+        <v>19</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B19">
+        <v>41</v>
+      </c>
+      <c r="C19">
         <v>19</v>
-      </c>
-      <c r="B19">
-        <v>34</v>
-      </c>
-      <c r="C19">
-        <v>15</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>20</v>
+        <v>34</v>
       </c>
       <c r="B20">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="C20">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>21</v>
+        <v>35</v>
       </c>
       <c r="B21">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="C21">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>22</v>
+        <v>36</v>
       </c>
       <c r="B22">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="C22">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>23</v>
+        <v>37</v>
       </c>
       <c r="B23">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="C23">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>24</v>
+        <v>38</v>
       </c>
       <c r="B24">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="C24">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>25</v>
+        <v>39</v>
       </c>
       <c r="B25">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="C25">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>26</v>
+        <v>40</v>
       </c>
       <c r="B26">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="C26">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>27</v>
+        <v>41</v>
       </c>
       <c r="B27">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="C27">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>28</v>
+        <v>42</v>
       </c>
       <c r="B28">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="C28">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>29</v>
+        <v>43</v>
       </c>
       <c r="B29">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="C29">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>30</v>
+        <v>44</v>
       </c>
       <c r="B30">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="C30">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>31</v>
+        <v>45</v>
       </c>
       <c r="B31">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="C31">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>32</v>
+        <v>46</v>
       </c>
       <c r="B32">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="C32">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>33</v>
+        <v>47</v>
       </c>
       <c r="B33">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="C33">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
       <c r="B34">
         <v>37</v>
@@ -2934,7 +2439,7 @@
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>35</v>
+        <v>49</v>
       </c>
       <c r="B35">
         <v>37</v>
@@ -2945,7 +2450,7 @@
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>36</v>
+        <v>50</v>
       </c>
       <c r="B36">
         <v>37</v>
@@ -2956,354 +2461,354 @@
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>37</v>
+        <v>2</v>
       </c>
       <c r="B37">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C37">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>38</v>
+        <v>3</v>
       </c>
       <c r="B38">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C38">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>39</v>
+        <v>4</v>
       </c>
       <c r="B39">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C39">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>40</v>
+        <v>5</v>
       </c>
       <c r="B40">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C40">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
-        <v>41</v>
+        <v>6</v>
       </c>
       <c r="B41">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C41">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
-        <v>42</v>
+        <v>7</v>
       </c>
       <c r="B42">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C42">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
-        <v>43</v>
+        <v>8</v>
       </c>
       <c r="B43">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C43">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
-        <v>44</v>
+        <v>9</v>
       </c>
       <c r="B44">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C44">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
-        <v>45</v>
+        <v>10</v>
       </c>
       <c r="B45">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C45">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
-        <v>46</v>
+        <v>11</v>
       </c>
       <c r="B46">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C46">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
-        <v>47</v>
+        <v>12</v>
       </c>
       <c r="B47">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C47">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
-        <v>48</v>
+        <v>13</v>
       </c>
       <c r="B48">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C48">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
-        <v>49</v>
+        <v>14</v>
       </c>
       <c r="B49">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C49">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
-        <v>50</v>
+        <v>15</v>
       </c>
       <c r="B50">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C50">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
-        <v>51</v>
+        <v>16</v>
       </c>
       <c r="B51">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="C51">
-        <v>19</v>
+        <v>14</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
-        <v>52</v>
+        <v>17</v>
       </c>
       <c r="B52">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="C52">
-        <v>19</v>
+        <v>14</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
-        <v>53</v>
+        <v>18</v>
       </c>
       <c r="B53">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="C53">
-        <v>19</v>
+        <v>14</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
-        <v>54</v>
+        <v>19</v>
       </c>
       <c r="B54">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="C54">
-        <v>19</v>
+        <v>15</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
-        <v>55</v>
+        <v>20</v>
       </c>
       <c r="B55">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="C55">
-        <v>19</v>
+        <v>15</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
-        <v>56</v>
+        <v>21</v>
       </c>
       <c r="B56">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="C56">
-        <v>19</v>
+        <v>15</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
-        <v>57</v>
+        <v>22</v>
       </c>
       <c r="B57">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="C57">
-        <v>19</v>
+        <v>15</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
-        <v>58</v>
+        <v>23</v>
       </c>
       <c r="B58">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="C58">
-        <v>19</v>
+        <v>15</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
-        <v>59</v>
+        <v>24</v>
       </c>
       <c r="B59">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="C59">
-        <v>19</v>
+        <v>15</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
-        <v>60</v>
+        <v>25</v>
       </c>
       <c r="B60">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="C60">
-        <v>19</v>
+        <v>15</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
-        <v>61</v>
+        <v>26</v>
       </c>
       <c r="B61">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="C61">
-        <v>19</v>
+        <v>15</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
-        <v>62</v>
+        <v>27</v>
       </c>
       <c r="B62">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="C62">
-        <v>19</v>
+        <v>15</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
-        <v>63</v>
+        <v>28</v>
       </c>
       <c r="B63">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="C63">
-        <v>19</v>
+        <v>15</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
-        <v>64</v>
+        <v>29</v>
       </c>
       <c r="B64">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="C64">
-        <v>19</v>
+        <v>15</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
-        <v>65</v>
+        <v>30</v>
       </c>
       <c r="B65">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="C65">
-        <v>19</v>
+        <v>15</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
-        <v>66</v>
+        <v>31</v>
       </c>
       <c r="B66">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="C66">
-        <v>19</v>
+        <v>15</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
-        <v>67</v>
+        <v>32</v>
       </c>
       <c r="B67">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="C67">
-        <v>19</v>
+        <v>15</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
-        <v>68</v>
+        <v>33</v>
       </c>
       <c r="B68">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="C68">
-        <v>19</v>
+        <v>15</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
@@ -3450,6 +2955,9 @@
       </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C81">
+    <sortCondition descending="1" ref="B3:B81"/>
+  </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>